<commit_message>
fix: excel baru liputan oap dan tod
</commit_message>
<xml_diff>
--- a/public/exports/LIPUTAN OAP.xlsx
+++ b/public/exports/LIPUTAN OAP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calypso\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6C59DF-9164-4401-8D49-7907AF80D67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761E9714-CA83-4CCA-B9B3-C97FE8D3116B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OA" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Negeri</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>% Liputan Penduduk Orang Asli</t>
-  </si>
-  <si>
-    <t>BAGI PERKHIDMATAN DI LUAR FASILITI KKM</t>
   </si>
   <si>
     <t xml:space="preserve">Anggaran Bilangan Penduduk Penan </t>
@@ -272,13 +269,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -567,6 +564,344 @@
   </sheetPr>
   <dimension ref="B1:G34"/>
   <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="E1" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="10" spans="2:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="9" t="e">
+        <f t="shared" ref="E11:E25" si="0">SUM(D11/C11)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>336</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4">
+        <v>61225</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4">
+        <v>20961</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4">
+        <v>12221</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1833</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <v>15825</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4">
+        <v>78615</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <v>17487</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1072</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="6">
+        <f>SUM(C19:C25)</f>
+        <v>112999</v>
+      </c>
+      <c r="D26" s="7">
+        <f>SUM(D11:D25)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" ref="E26" si="1">SUM(D26/C26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:G17"/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
@@ -583,403 +918,61 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E1" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="B6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="10" spans="2:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="9" t="e">
-        <f t="shared" ref="E11:E25" si="0">SUM(D11/C11)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3">
-        <v>336</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="4">
-        <v>61225</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="4">
-        <v>20961</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="4">
-        <v>12221</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1833</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4">
-        <v>15825</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="4">
-        <v>78615</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4">
-        <v>17487</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1072</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="6">
-        <f>SUM(C19:C25)</f>
-        <v>112999</v>
-      </c>
-      <c r="D26" s="7">
-        <f>SUM(D11:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="10">
-        <f t="shared" ref="E26" si="1">SUM(D26/C26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B7:E7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="88" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="B1:G17"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="E1" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="10" spans="2:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>13</v>
@@ -1020,20 +1013,20 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>